<commit_message>
heatplot Removed sample 19
</commit_message>
<xml_diff>
--- a/Data/unique for HFD XN.xlsx
+++ b/Data/unique for HFD XN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trant\Desktop\FXR\Fxr\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kioussilab/Desktop/FXR analysis/Fxr/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EC09792-E98C-4FF2-9A84-B51CFA9C8007}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A1F4C6-4E4A-B647-89CB-AF31CBF363D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="5900" yWindow="2600" windowWidth="47040" windowHeight="23220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unique for HFD XN" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="191">
   <si>
     <t>log2FC.HFD</t>
   </si>
@@ -539,12 +539,76 @@
   </si>
   <si>
     <t>Gm3435</t>
+  </si>
+  <si>
+    <t>(1) Cathepsin E-deficient mice show increased susceptibility to bacterial infection associated with the decreased expression of multiple cell surface Toll-like receptors.
+Tsukuba T, Yamamoto S, Yanagawa M, Okamoto K, Okamoto Y, Nakayama KI, Kadowaki T, Yamamoto K
+J Biochem. 2006 Jul; 140(1):57-66.
+(2) An immunocytochemical study on distinct intracellular localization of cathepsin E and cathepsin D in human gastric cells and various rat cells.
+Saku T, Sakai H, Shibata Y, Kato Y, Yamamoto K
+J Biochem. 1991 Dec; 110(6):956-64.</t>
+  </si>
+  <si>
+    <t>(1) Generally involved in inflammatory response and infection. Found to be significantly upregulated hepatocellular carcinomas
+(2) Saku et al. demonstrated expression of CTSE localized within the bile canaliculi of the rat liver as well as microvilli of hepatic cells</t>
+  </si>
+  <si>
+    <t>(3) promote white adipogenesis and fat storage
+(4) Ifi202b modulates fat accumulation through expression of adipogenic genes such as 11β-Hsd1.</t>
+  </si>
+  <si>
+    <t>(3) Stadion, M. et al. Increased Ifi202b/IFI16 expression stimulates adipogenesis in mice and humans. Diabetologia 61, 1167–1179 (2018).
+(4) Vogel, H. et al. Loss of function of Ifi202b by a microdeletion on chromosome 1 of C57BL/6J mice suppresses 11β-hydroxysteroid dehydrogenase type 1 expression and development of obesity. Hum. Mol. Genet. 21, 3845–3857 (2012).</t>
+  </si>
+  <si>
+    <t>(5) Timp1 is upregulated in liver cirrhosis and liver cancer but not essential in hepatic fibrogenesis and carcinogenesis in mice
+(6) Timp1 is upregulated following acute/chronic liver injury. Plays a direct role in inhibition of ECM proteolysis and indirect role in ECM turnover rate</t>
+  </si>
+  <si>
+    <t>(5) Thiele, N. D. et al. TIMP-1 is upregulated, but not essential in hepatic fibrogenesis and carcinogenesis in mice. Sci. Rep. 7, (2017).
+(6) Wang, H. et al. Tissue inhibitor of metalloproteinase 1 (TIMP-1) deficiency exacerbates carbon tetrachloride-induced liver injury and fibrosis in mice: involvement of hepatocyte STAT3 in TIMP-1 production. Cell Biosci. 1, 14 (2011).</t>
+  </si>
+  <si>
+    <t>(7) Evelated level of Saa2 is associated with insulin resistance. Mice fed with HFD show significantly increased level of Saa2</t>
+  </si>
+  <si>
+    <t>(7) Scheja, L. et al. Acute-Phase Serum Amyloid A as a Marker of Insulin Resistance in Mice. Journal of Diabetes Research https://www.hindawi.com/journals/jdr/2008/230837/ (2008) doi:10.1155/2008/230837.</t>
+  </si>
+  <si>
+    <t>(8) Cdca7l can activate the extracellular signal-regulated kinase 1/2 (ERK1/2) signaling pathway and regulated the cell cycle, thus promoting hepatocellular carcinomas progression</t>
+  </si>
+  <si>
+    <t>(8) Tian, Y. et al. CDCA7L promotes hepatocellular carcinoma progression by regulating the cell cycle. Int. J. Oncol. 43, 2082–2090 (2013).</t>
+  </si>
+  <si>
+    <t>(9) knocking out this genes stabilizes LXR and reduce both atherosclerosis and steatohepatitis</t>
+  </si>
+  <si>
+    <t>(9) Hsieh, J. et al. TTC39B deficiency stabilizes LXR reducing both atherosclerosis and steatohepatitis. Nature 535, 303–307 (2016).</t>
+  </si>
+  <si>
+    <t>(10) regulated by FXR, involved in inflammatory response. Tissue and species-specific</t>
+  </si>
+  <si>
+    <t>(10) Porez, G. et al. The Hepatic Orosomucoid/α1-Acid Glycoprotein Gene Cluster Is Regulated by the Nuclear Bile Acid Receptor FXR. Endocrinology 154, 3690–3701 (2013).</t>
+  </si>
+  <si>
+    <t>(11) Goi, T., Nakazawa, T., Hirono, Y. &amp; Yamaguchi, A. The anti-tumor effect is enhanced by simultaneously targeting VEGF and PROK1 in colorectal cancer. Oncotarget 6, 6053–6061 (2015).</t>
+  </si>
+  <si>
+    <t>(11) suppressing of Prok1 and VEGF simutaneously results in anti-tumor effect in colorectal cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(12) regulates phagocytosis and cytokin production in Kupffer cells during liver injury. Helps alleviate liver fibrosis and heal injury </t>
+  </si>
+  <si>
+    <t>(12) Miyazaki, H. et al. Fatty acid binding protein 7 regulates phagocytosis and cytokine production in Kupffer cells during liver injury. Am. J. Pathol. 184, 2505–2515 (2014).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1022,8 +1086,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1378,1891 +1448,1954 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C171"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="8.83203125" style="2"/>
+    <col min="4" max="4" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="101" style="1" customWidth="1"/>
+    <col min="6" max="6" width="119.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
         <v>4.7280650660000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
         <v>3.5997058210000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
         <v>3.5630432079999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
         <v>2.5881593060000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
         <v>2.581784029</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="E6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
         <v>2.4934058179999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
         <v>2.261322367</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="E8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
         <v>2.0636519660000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="E9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
         <v>1.9020362310000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
         <v>1.8766216200000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
         <v>1.857231984</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
         <v>1.8400752149999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
         <v>1.821935452</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
         <v>1.8189852950000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
         <v>1.7907371059999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
         <v>1.7591424229999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="E17" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
         <v>1.7292535499999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
         <v>1.683277007</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
         <v>1.6611374759999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
         <v>1.6406469530000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2">
         <v>1.615603772</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2">
         <v>1.5545572089999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
         <v>1.5524019630000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
         <v>1.5172256</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
         <v>1.508611132</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
         <v>1.5041204969999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
         <v>1.4827921420000001</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2">
         <v>1.481495056</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2">
         <v>1.4712354329999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2">
         <v>1.4563592139999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2">
         <v>1.4491904879999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2">
         <v>1.4373321999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
         <v>1.427675397</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2">
         <v>1.4238313499999999</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2">
         <v>1.4100749889999999</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37">
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2">
         <v>1.409892264</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38">
+      <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2">
         <v>1.405955474</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39">
+      <c r="B39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2">
         <v>1.405666587</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40">
+      <c r="B40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2">
         <v>1.40155265</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2">
         <v>1.391990807</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42">
+      <c r="B42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2">
         <v>1.3730403149999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43">
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2">
         <v>1.3547070400000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2">
         <v>1.3543091389999999</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2">
         <v>1.353208891</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46">
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2">
         <v>1.34763459</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47">
+      <c r="B47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2">
         <v>1.3265613810000001</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48">
+      <c r="B48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2">
         <v>1.296176821</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49">
+      <c r="B49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2">
         <v>1.289370141</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50">
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="2">
         <v>1.2846035689999999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51">
+      <c r="B51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="2">
         <v>1.2808277800000001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52">
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="2">
         <v>1.276046327</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53">
+      <c r="B53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2">
         <v>1.266991725</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2">
         <v>1.2667203039999999</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55">
+      <c r="B55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="2">
         <v>1.2663321350000001</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56">
+      <c r="B56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="2">
         <v>1.2627795829999999</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57">
+      <c r="B57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2">
         <v>1.258162469</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B58" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58">
+      <c r="B58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="2">
         <v>1.255750082</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B59" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59">
+      <c r="B59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="2">
         <v>1.2554124419999999</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60">
+      <c r="B60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="2">
         <v>1.2550728959999999</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B61" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61">
+      <c r="B61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="2">
         <v>1.2483093249999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B62" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62">
+      <c r="B62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2">
         <v>1.244019304</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B63" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63">
+      <c r="B63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="2">
         <v>1.2388768800000001</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64">
+      <c r="B64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="2">
         <v>1.230921433</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65">
+      <c r="B65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="2">
         <v>1.218975777</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66">
+      <c r="B66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="2">
         <v>1.2059728059999999</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67">
+      <c r="B67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="2">
         <v>1.194060565</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B68" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68">
+      <c r="B68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2">
         <v>1.1833899720000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B69" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69">
+      <c r="B69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="2">
         <v>1.1574945130000001</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70">
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="2">
         <v>1.1555500219999999</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71">
+      <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="2">
         <v>1.154558967</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72">
+      <c r="B72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="2">
         <v>1.154151068</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73">
+      <c r="B73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="2">
         <v>1.1513017640000001</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74">
+      <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="2">
         <v>1.130846427</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B75" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75">
+      <c r="B75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="2">
         <v>1.1237260840000001</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76">
+      <c r="B76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="2">
         <v>1.108788385</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77">
+      <c r="B77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="2">
         <v>1.106552553</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B78" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78">
+      <c r="B78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="2">
         <v>1.0929700389999999</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79">
+      <c r="B79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="2">
         <v>1.0927002299999999</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B80" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80">
+      <c r="B80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="2">
         <v>1.088620559</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81">
+      <c r="B81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="2">
         <v>1.0750886310000001</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82">
+      <c r="B82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="2">
         <v>1.0731607409999999</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B83" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83">
+      <c r="B83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="2">
         <v>1.0509476680000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B84" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84">
+      <c r="B84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="2">
         <v>1.0387805670000001</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B85" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85">
+      <c r="B85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="2">
         <v>1.0106545950000001</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B86" t="s">
-        <v>3</v>
-      </c>
-      <c r="C86">
+      <c r="B86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="2">
         <v>1.0053313399999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B87" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87">
+      <c r="B87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="2">
         <v>0.99815759500000001</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88">
+      <c r="B88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="2">
         <v>0.95558879600000002</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B89" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89">
+      <c r="B89" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" s="2">
         <v>0.95303737200000005</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B90" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90">
+      <c r="B90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="2">
         <v>0.95151460700000001</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B91" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91">
+      <c r="B91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="2">
         <v>0.94427037899999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B92" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92">
+      <c r="B92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="2">
         <v>0.92816248400000001</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B93" t="s">
-        <v>3</v>
-      </c>
-      <c r="C93">
+      <c r="B93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="2">
         <v>0.91561183599999996</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B94" t="s">
-        <v>3</v>
-      </c>
-      <c r="C94">
+      <c r="B94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="2">
         <v>0.91534807699999998</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="95" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B95" t="s">
-        <v>3</v>
-      </c>
-      <c r="C95">
+      <c r="B95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="2">
         <v>0.89390811000000003</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B96" t="s">
-        <v>3</v>
-      </c>
-      <c r="C96">
+      <c r="B96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="2">
         <v>0.89213267900000004</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="97" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B97" t="s">
-        <v>3</v>
-      </c>
-      <c r="C97">
+      <c r="B97" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="2">
         <v>0.88870423899999995</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="98" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B98" t="s">
-        <v>3</v>
-      </c>
-      <c r="C98">
+      <c r="B98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" s="2">
         <v>0.87783376400000002</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="99" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B99" t="s">
-        <v>3</v>
-      </c>
-      <c r="C99">
+      <c r="B99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="2">
         <v>0.857856375</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="100" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B100" t="s">
-        <v>3</v>
-      </c>
-      <c r="C100">
+      <c r="B100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="2">
         <v>0.83415086299999996</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="101" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B101" t="s">
-        <v>3</v>
-      </c>
-      <c r="C101">
+      <c r="B101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="2">
         <v>0.83133639999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row r="102" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B102" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102">
+      <c r="B102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="2">
         <v>0.77699604200000005</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row r="103" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B103" t="s">
-        <v>3</v>
-      </c>
-      <c r="C103">
+      <c r="B103" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="2">
         <v>0.77380081700000003</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B104" t="s">
-        <v>3</v>
-      </c>
-      <c r="C104">
+      <c r="B104" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" s="2">
         <v>0.65389775100000003</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="105" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B105" t="s">
-        <v>3</v>
-      </c>
-      <c r="C105">
+      <c r="B105" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="2">
         <v>0.62460631099999997</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B106" t="s">
-        <v>3</v>
-      </c>
-      <c r="C106">
+      <c r="B106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106" s="2">
         <v>0.61795056599999998</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B107" t="s">
-        <v>3</v>
-      </c>
-      <c r="C107">
+      <c r="B107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" s="2">
         <v>0.61210016099999998</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B108" t="s">
-        <v>3</v>
-      </c>
-      <c r="C108">
+      <c r="B108" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="2">
         <v>0.55240623</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B109" t="s">
-        <v>3</v>
-      </c>
-      <c r="C109">
+      <c r="B109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C109" s="2">
         <v>0.25977313699999999</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B110" t="s">
-        <v>3</v>
-      </c>
-      <c r="C110">
+      <c r="B110" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" s="2">
         <v>0.18928947700000001</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B111" t="s">
-        <v>3</v>
-      </c>
-      <c r="C111">
+      <c r="B111" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" s="2">
         <v>-0.59940848499999999</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+    <row r="112" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B112" t="s">
-        <v>3</v>
-      </c>
-      <c r="C112">
+      <c r="B112" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="2">
         <v>-0.62977482500000004</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row r="113" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B113" t="s">
-        <v>3</v>
-      </c>
-      <c r="C113">
+      <c r="B113" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" s="2">
         <v>-0.65070305100000003</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B114" t="s">
-        <v>3</v>
-      </c>
-      <c r="C114">
+      <c r="B114" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C114" s="2">
         <v>-0.68762346900000004</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B115" t="s">
-        <v>3</v>
-      </c>
-      <c r="C115">
+      <c r="B115" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" s="2">
         <v>-0.71412825499999999</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+    <row r="116" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B116" t="s">
-        <v>3</v>
-      </c>
-      <c r="C116">
+      <c r="B116" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116" s="2">
         <v>-0.74803223399999996</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+    <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B117" t="s">
-        <v>3</v>
-      </c>
-      <c r="C117">
+      <c r="B117" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117" s="2">
         <v>-0.74967020399999995</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+    <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B118" t="s">
-        <v>3</v>
-      </c>
-      <c r="C118">
+      <c r="B118" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" s="2">
         <v>-0.75648371800000003</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row r="119" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B119" t="s">
-        <v>3</v>
-      </c>
-      <c r="C119">
+      <c r="B119" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" s="2">
         <v>-0.773167787</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+    <row r="120" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" t="s">
-        <v>3</v>
-      </c>
-      <c r="C120">
+      <c r="B120" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" s="2">
         <v>-0.78182189000000002</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+    <row r="121" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B121" t="s">
-        <v>3</v>
-      </c>
-      <c r="C121">
+      <c r="B121" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" s="2">
         <v>-0.78531771699999997</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+    <row r="122" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B122" t="s">
-        <v>3</v>
-      </c>
-      <c r="C122">
+      <c r="B122" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" s="2">
         <v>-0.79307777700000004</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+    <row r="123" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B123" t="s">
-        <v>3</v>
-      </c>
-      <c r="C123">
+      <c r="B123" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123" s="2">
         <v>-0.812518356</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+    <row r="124" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B124" t="s">
-        <v>3</v>
-      </c>
-      <c r="C124">
+      <c r="B124" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124" s="2">
         <v>-0.82267886700000004</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+    <row r="125" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B125" t="s">
-        <v>3</v>
-      </c>
-      <c r="C125">
+      <c r="B125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" s="2">
         <v>-0.84099836100000003</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+    <row r="126" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B126" t="s">
-        <v>3</v>
-      </c>
-      <c r="C126">
+      <c r="B126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C126" s="2">
         <v>-0.87322949699999997</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+    <row r="127" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B127" t="s">
-        <v>3</v>
-      </c>
-      <c r="C127">
+      <c r="B127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" s="2">
         <v>-0.87524746099999995</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+    <row r="128" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B128" t="s">
-        <v>3</v>
-      </c>
-      <c r="C128">
+      <c r="B128" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C128" s="2">
         <v>-0.90103575700000005</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+    <row r="129" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B129" t="s">
-        <v>3</v>
-      </c>
-      <c r="C129">
+      <c r="B129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129" s="2">
         <v>-0.91815100100000002</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+    <row r="130" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B130" t="s">
-        <v>3</v>
-      </c>
-      <c r="C130">
+      <c r="B130" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130" s="2">
         <v>-0.92593940799999996</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+    <row r="131" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B131" t="s">
-        <v>3</v>
-      </c>
-      <c r="C131">
+      <c r="B131" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131" s="2">
         <v>-0.94899342900000005</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+    <row r="132" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B132" t="s">
-        <v>3</v>
-      </c>
-      <c r="C132">
+      <c r="B132" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C132" s="2">
         <v>-0.95425984500000005</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+    <row r="133" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B133" t="s">
-        <v>3</v>
-      </c>
-      <c r="C133">
+      <c r="B133" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" s="2">
         <v>-0.97246614899999995</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+    <row r="134" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B134" t="s">
-        <v>3</v>
-      </c>
-      <c r="C134">
+      <c r="B134" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C134" s="2">
         <v>-0.98254125299999995</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+    <row r="135" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B135" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135">
+      <c r="B135" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135" s="2">
         <v>-1.015689756</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+    <row r="136" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B136" t="s">
-        <v>3</v>
-      </c>
-      <c r="C136">
+      <c r="B136" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" s="2">
         <v>-1.0270692459999999</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+    <row r="137" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B137" t="s">
-        <v>3</v>
-      </c>
-      <c r="C137">
+      <c r="B137" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" s="2">
         <v>-1.042710263</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+    <row r="138" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B138" t="s">
-        <v>3</v>
-      </c>
-      <c r="C138">
+      <c r="B138" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C138" s="2">
         <v>-1.0468336680000001</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+    <row r="139" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B139" t="s">
-        <v>3</v>
-      </c>
-      <c r="C139">
+      <c r="B139" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C139" s="2">
         <v>-1.0506999610000001</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+    <row r="140" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B140" t="s">
-        <v>3</v>
-      </c>
-      <c r="C140">
+      <c r="B140" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" s="2">
         <v>-1.088000536</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+    <row r="141" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B141" t="s">
-        <v>3</v>
-      </c>
-      <c r="C141">
+      <c r="B141" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" s="2">
         <v>-1.1197467409999999</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+    <row r="142" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B142" t="s">
-        <v>3</v>
-      </c>
-      <c r="C142">
+      <c r="B142" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" s="2">
         <v>-1.129535706</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+    <row r="143" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B143" t="s">
-        <v>3</v>
-      </c>
-      <c r="C143">
+      <c r="B143" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143" s="2">
         <v>-1.1412507780000001</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+    <row r="144" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B144" t="s">
-        <v>3</v>
-      </c>
-      <c r="C144">
+      <c r="B144" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" s="2">
         <v>-1.1420138099999999</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+    <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B145" t="s">
-        <v>3</v>
-      </c>
-      <c r="C145">
+      <c r="B145" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C145" s="2">
         <v>-1.229413616</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+    <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B146" t="s">
-        <v>3</v>
-      </c>
-      <c r="C146">
+      <c r="B146" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C146" s="2">
         <v>-1.2557470559999999</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+    <row r="147" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B147" t="s">
-        <v>3</v>
-      </c>
-      <c r="C147">
+      <c r="B147" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147" s="2">
         <v>-1.281222504</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+    <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B148" t="s">
-        <v>3</v>
-      </c>
-      <c r="C148">
+      <c r="B148" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148" s="2">
         <v>-1.3085835770000001</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+    <row r="149" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B149" t="s">
-        <v>3</v>
-      </c>
-      <c r="C149">
+      <c r="B149" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" s="2">
         <v>-1.314228441</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+    <row r="150" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B150" t="s">
-        <v>3</v>
-      </c>
-      <c r="C150">
+      <c r="B150" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C150" s="2">
         <v>-1.332970041</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+    <row r="151" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B151" t="s">
-        <v>3</v>
-      </c>
-      <c r="C151">
+      <c r="B151" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" s="2">
         <v>-1.3582055710000001</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
+    <row r="152" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B152" t="s">
-        <v>3</v>
-      </c>
-      <c r="C152">
+      <c r="B152" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" s="2">
         <v>-1.369225248</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
+    <row r="153" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B153" t="s">
-        <v>3</v>
-      </c>
-      <c r="C153">
+      <c r="B153" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" s="2">
         <v>-1.382462651</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+    <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B154" t="s">
-        <v>3</v>
-      </c>
-      <c r="C154">
+      <c r="B154" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154" s="2">
         <v>-1.391955582</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+    <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B155" t="s">
-        <v>3</v>
-      </c>
-      <c r="C155">
+      <c r="B155" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" s="2">
         <v>-1.4067033470000001</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+    <row r="156" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B156" t="s">
-        <v>3</v>
-      </c>
-      <c r="C156">
+      <c r="B156" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" s="2">
         <v>-1.4072611989999999</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
+    <row r="157" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B157" t="s">
-        <v>3</v>
-      </c>
-      <c r="C157">
+      <c r="B157" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" s="2">
         <v>-1.4298899970000001</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+    <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B158" t="s">
-        <v>3</v>
-      </c>
-      <c r="C158">
+      <c r="B158" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" s="2">
         <v>-1.4568912890000001</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
+    <row r="159" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B159" t="s">
-        <v>3</v>
-      </c>
-      <c r="C159">
+      <c r="B159" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" s="2">
         <v>-1.472837119</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+    <row r="160" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B160" t="s">
-        <v>3</v>
-      </c>
-      <c r="C160">
+      <c r="B160" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="2">
         <v>-1.5192216890000001</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+    <row r="161" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B161" t="s">
-        <v>3</v>
-      </c>
-      <c r="C161">
+      <c r="B161" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161" s="2">
         <v>-1.5200252160000001</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B162" t="s">
-        <v>3</v>
-      </c>
-      <c r="C162">
+      <c r="B162" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C162" s="2">
         <v>-1.6212192139999999</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B163" t="s">
-        <v>3</v>
-      </c>
-      <c r="C163">
+      <c r="B163" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163" s="2">
         <v>-1.653710856</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
+    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B164" t="s">
-        <v>3</v>
-      </c>
-      <c r="C164">
+      <c r="B164" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164" s="2">
         <v>-1.715439274</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B165" t="s">
-        <v>3</v>
-      </c>
-      <c r="C165">
+      <c r="B165" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C165" s="2">
         <v>-1.7410179560000001</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
+    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B166" t="s">
-        <v>3</v>
-      </c>
-      <c r="C166">
+      <c r="B166" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C166" s="2">
         <v>-1.9186905059999999</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+    <row r="167" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B167" t="s">
-        <v>3</v>
-      </c>
-      <c r="C167">
+      <c r="B167" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C167" s="2">
         <v>-1.9245523879999999</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
+    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B168" t="s">
-        <v>3</v>
-      </c>
-      <c r="C168">
+      <c r="B168" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C168" s="2">
         <v>-1.9245523879999999</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B169" t="s">
-        <v>3</v>
-      </c>
-      <c r="C169">
+      <c r="B169" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C169" s="2">
         <v>-2.0232827019999999</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
+    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B170" t="s">
-        <v>3</v>
-      </c>
-      <c r="C170">
+      <c r="B170" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C170" s="2">
         <v>-2.2706605880000001</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+    <row r="171" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B171" t="s">
-        <v>3</v>
-      </c>
-      <c r="C171">
+      <c r="B171" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C171" s="2">
         <v>-2.6956978540000001</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>